<commit_message>
more images and video
</commit_message>
<xml_diff>
--- a/docs/data/data_prep/family_data.xlsx
+++ b/docs/data/data_prep/family_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savch\Google Drive\Work\Family-tree_v8 - reduced number of cells\web\data\data_prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123B31CE-A0D7-4237-9EAF-10C31ABF9BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002F143C-E716-4825-9FDA-34689B075DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="286">
   <si>
     <t>PersonID</t>
   </si>
@@ -875,6 +875,9 @@
   </si>
   <si>
     <t>Хасын, Магаданская область, Россия</t>
+  </si>
+  <si>
+    <t>id4-dima.png</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1243,7 @@
   <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,6 +1473,9 @@
       <c r="P5" t="s">
         <v>47</v>
       </c>
+      <c r="Q5" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>

<commit_message>
new people and details
</commit_message>
<xml_diff>
--- a/docs/data/data_prep/family_data.xlsx
+++ b/docs/data/data_prep/family_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents (Disk D)\Google Drive (Disk D)\Work\Family-tree_v6 - github\web\docs\data\data_prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A2C6C7-EDEA-426D-AD6A-139CCF0EB220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F077901B-2CC8-404B-8003-6EA0C122F6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1740" windowWidth="26475" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2175" windowWidth="15060" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FamilyData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="325">
   <si>
     <t>PersonID</t>
   </si>
@@ -34,6 +34,9 @@
     <t>LastName-ru</t>
   </si>
   <si>
+    <t>Maiden_name</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -196,6 +199,9 @@
     <t>Анна-София</t>
   </si>
   <si>
+    <t>Мельникова</t>
+  </si>
+  <si>
     <t>18.01.1983</t>
   </si>
   <si>
@@ -268,9 +274,6 @@
     <t>Милана</t>
   </si>
   <si>
-    <t>Мельникова</t>
-  </si>
-  <si>
     <t>id11-milana.png</t>
   </si>
   <si>
@@ -301,6 +304,9 @@
     <t>Королёва</t>
   </si>
   <si>
+    <t>Пашкова</t>
+  </si>
+  <si>
     <t>21.05.1966</t>
   </si>
   <si>
@@ -388,9 +394,6 @@
     <t>Виктория</t>
   </si>
   <si>
-    <t>Пашкова</t>
-  </si>
-  <si>
     <t>28.12.1968</t>
   </si>
   <si>
@@ -529,6 +532,9 @@
     <t>Лилина</t>
   </si>
   <si>
+    <t>Лапцевич</t>
+  </si>
+  <si>
     <t>11.10.1928</t>
   </si>
   <si>
@@ -571,6 +577,9 @@
     <t>Котлинская</t>
   </si>
   <si>
+    <t>66, 67, 68, 69, 70</t>
+  </si>
+  <si>
     <t>29, 33, 34, 35</t>
   </si>
   <si>
@@ -583,10 +592,7 @@
     <t>Василий</t>
   </si>
   <si>
-    <t>Лапцевич</t>
-  </si>
-  <si>
-    <t>52</t>
+    <t>61, 52, 62, 63, 64, 65</t>
   </si>
   <si>
     <t>id32-vasilii.png</t>
@@ -832,7 +838,7 @@
     <t>id51-kazimir.png</t>
   </si>
   <si>
-    <t>32</t>
+    <t>32,  62, 63, 64, 65, 61</t>
   </si>
   <si>
     <t>Наша мама о нём отзывалась как об очень мудром и умном человеком.</t>
@@ -896,6 +902,99 @@
   </si>
   <si>
     <t>Устинья</t>
+  </si>
+  <si>
+    <t>Moisei</t>
+  </si>
+  <si>
+    <t>Моисей</t>
+  </si>
+  <si>
+    <t>32, 52, 62, 63, 64, 65</t>
+  </si>
+  <si>
+    <t>Gavriil</t>
+  </si>
+  <si>
+    <t>Гавриил</t>
+  </si>
+  <si>
+    <t>32, 52, 61, 63, 64, 65</t>
+  </si>
+  <si>
+    <t>Michail</t>
+  </si>
+  <si>
+    <t>32, 52, 61, 62, 64, 65</t>
+  </si>
+  <si>
+    <t>Evdokia</t>
+  </si>
+  <si>
+    <t>Евдокия</t>
+  </si>
+  <si>
+    <t>32, 52, 61, 62, 63, 65</t>
+  </si>
+  <si>
+    <t>Domna</t>
+  </si>
+  <si>
+    <t>Домна</t>
+  </si>
+  <si>
+    <t>32, 52, 61, 62, 63, 64</t>
+  </si>
+  <si>
+    <t>Kuzma</t>
+  </si>
+  <si>
+    <t>Кузьма</t>
+  </si>
+  <si>
+    <t>31, 67, 68, 69, 70</t>
+  </si>
+  <si>
+    <t>31, 66, 68, 69, 70</t>
+  </si>
+  <si>
+    <t>Antonina</t>
+  </si>
+  <si>
+    <t>Антонина</t>
+  </si>
+  <si>
+    <t>Тарасевич</t>
+  </si>
+  <si>
+    <t>31, 66, 67, 69, 70</t>
+  </si>
+  <si>
+    <t>Agrippina</t>
+  </si>
+  <si>
+    <t>Агриппина</t>
+  </si>
+  <si>
+    <t>Кульпанович</t>
+  </si>
+  <si>
+    <t>31, 66, 67, 68, 70</t>
+  </si>
+  <si>
+    <t>Lubov</t>
+  </si>
+  <si>
+    <t>Любовь</t>
+  </si>
+  <si>
+    <t>Соловей</t>
+  </si>
+  <si>
+    <t>31, 66, 67, 68, 69</t>
+  </si>
+  <si>
+    <t>30.11.1959</t>
   </si>
 </sst>
 </file>
@@ -1258,15 +1357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1321,46 +1420,46 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
         <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="H2">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>27</v>
       </c>
-      <c r="J2">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
+      <c r="K2">
+        <v>28</v>
       </c>
       <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2">
         <v>4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
       </c>
       <c r="O2" t="s">
         <v>26</v>
@@ -1368,81 +1467,81 @@
       <c r="P2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="H3">
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3">
         <v>4</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
       </c>
       <c r="P3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4">
         <v>21</v>
       </c>
-      <c r="J4">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4">
+      <c r="K4">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
-        <v>25</v>
-      </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="P4" t="s">
         <v>39</v>
@@ -1450,40 +1549,40 @@
       <c r="Q4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5">
         <v>21</v>
       </c>
-      <c r="J5">
-        <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5">
+      <c r="K5">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5">
         <v>5</v>
-      </c>
-      <c r="N5" t="s">
-        <v>45</v>
       </c>
       <c r="O5" t="s">
         <v>46</v>
@@ -1494,2187 +1593,2576 @@
       <c r="Q5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6">
         <v>6</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>21</v>
       </c>
-      <c r="J6">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>52</v>
+      <c r="K6">
+        <v>22</v>
       </c>
       <c r="L6" t="s">
         <v>53</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="P6" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="Q6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="R6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>10</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>11</v>
       </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
       <c r="L7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7">
         <v>5</v>
       </c>
-      <c r="N7" t="s">
-        <v>60</v>
-      </c>
       <c r="O7" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="P7" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="Q7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8">
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>6</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>6</v>
       </c>
-      <c r="N8" t="s">
-        <v>65</v>
-      </c>
       <c r="O8" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="P8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="Q8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9">
         <v>9</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>11</v>
       </c>
-      <c r="K9" t="s">
-        <v>69</v>
-      </c>
       <c r="L9" t="s">
-        <v>70</v>
-      </c>
-      <c r="M9">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9">
         <v>5</v>
       </c>
-      <c r="O9" t="s">
-        <v>71</v>
-      </c>
       <c r="P9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="M10" t="s">
         <v>72</v>
       </c>
-      <c r="C10" t="s">
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
         <v>73</v>
       </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
-      <c r="L10" t="s">
-        <v>70</v>
-      </c>
-      <c r="M10">
-        <v>5</v>
-      </c>
-      <c r="O10" t="s">
-        <v>71</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11">
         <v>11</v>
       </c>
-      <c r="L11" t="s">
-        <v>78</v>
-      </c>
-      <c r="M11">
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11">
         <v>4</v>
       </c>
-      <c r="O11" t="s">
-        <v>79</v>
-      </c>
       <c r="P11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="P12" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12">
-        <v>10</v>
-      </c>
-      <c r="L12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12">
-        <v>4</v>
-      </c>
-      <c r="O12" t="s">
-        <v>79</v>
-      </c>
-      <c r="P12" t="s">
-        <v>27</v>
-      </c>
       <c r="Q12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13">
+        <v>86</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13">
         <v>9</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>8</v>
       </c>
-      <c r="K13" t="s">
-        <v>86</v>
-      </c>
-      <c r="M13">
+      <c r="L13" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13">
         <v>6</v>
       </c>
-      <c r="O13" t="s">
-        <v>71</v>
-      </c>
       <c r="P13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14">
         <v>9</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>8</v>
       </c>
-      <c r="K14" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14">
+      <c r="L14" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14">
         <v>6</v>
       </c>
-      <c r="O14" t="s">
-        <v>71</v>
-      </c>
       <c r="P14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15">
-        <v>15</v>
-      </c>
-      <c r="I15">
-        <v>30</v>
-      </c>
-      <c r="J15">
+      <c r="K15">
         <v>29</v>
       </c>
-      <c r="K15" t="s">
-        <v>94</v>
-      </c>
       <c r="L15" t="s">
-        <v>95</v>
-      </c>
-      <c r="M15">
+        <v>96</v>
+      </c>
+      <c r="M15" t="s">
+        <v>97</v>
+      </c>
+      <c r="N15">
         <v>4</v>
       </c>
-      <c r="N15" t="s">
-        <v>96</v>
-      </c>
       <c r="O15" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="P15" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q15" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="R15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="S15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16">
         <v>14</v>
       </c>
-      <c r="L16" t="s">
-        <v>95</v>
-      </c>
-      <c r="M16">
+      <c r="M16" t="s">
+        <v>97</v>
+      </c>
+      <c r="N16">
         <v>4</v>
       </c>
-      <c r="N16" t="s">
-        <v>96</v>
-      </c>
       <c r="O16" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="P16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H17">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17">
         <v>24</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>15</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>14</v>
       </c>
-      <c r="K17" t="s">
-        <v>105</v>
-      </c>
       <c r="L17" t="s">
-        <v>106</v>
-      </c>
-      <c r="M17">
+        <v>107</v>
+      </c>
+      <c r="M17" t="s">
+        <v>108</v>
+      </c>
+      <c r="N17">
         <v>5</v>
       </c>
-      <c r="N17" t="s">
-        <v>96</v>
-      </c>
       <c r="O17" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="P17" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q17" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="R17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="S17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
-      </c>
-      <c r="I18">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18">
         <v>15</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>14</v>
       </c>
-      <c r="K18" t="s">
-        <v>112</v>
-      </c>
-      <c r="M18">
+      <c r="L18" t="s">
+        <v>114</v>
+      </c>
+      <c r="N18">
         <v>5</v>
       </c>
-      <c r="N18" t="s">
-        <v>38</v>
-      </c>
       <c r="O18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19">
         <v>19</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>30</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>29</v>
       </c>
-      <c r="K19" t="s">
-        <v>115</v>
-      </c>
       <c r="L19" t="s">
-        <v>116</v>
-      </c>
-      <c r="M19">
+        <v>117</v>
+      </c>
+      <c r="M19" t="s">
+        <v>118</v>
+      </c>
+      <c r="N19">
         <v>4</v>
       </c>
-      <c r="N19" t="s">
-        <v>117</v>
-      </c>
       <c r="O19" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="P19" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q19" t="s">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="R19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="S19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H20">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>124</v>
+      </c>
+      <c r="I20">
         <v>18</v>
       </c>
-      <c r="L20" t="s">
-        <v>116</v>
-      </c>
-      <c r="M20">
+      <c r="M20" t="s">
+        <v>118</v>
+      </c>
+      <c r="N20">
         <v>4</v>
       </c>
-      <c r="O20" t="s">
-        <v>38</v>
-      </c>
       <c r="P20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="F21" t="s">
-        <v>124</v>
-      </c>
-      <c r="I21">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21">
         <v>18</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>19</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>5</v>
       </c>
-      <c r="P21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
         <v>21</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H22">
-        <v>22</v>
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>128</v>
       </c>
       <c r="I22">
+        <v>22</v>
+      </c>
+      <c r="J22">
         <v>27</v>
       </c>
-      <c r="J22">
-        <v>28</v>
-      </c>
-      <c r="K22" t="s">
-        <v>128</v>
+      <c r="K22">
+        <v>28</v>
       </c>
       <c r="L22" t="s">
         <v>129</v>
       </c>
-      <c r="M22">
+      <c r="M22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N22">
         <v>4</v>
       </c>
-      <c r="N22" t="s">
-        <v>25</v>
-      </c>
       <c r="O22" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="P22" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="Q22" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <v>30</v>
+      </c>
+      <c r="K23">
+        <v>29</v>
+      </c>
+      <c r="L23" t="s">
+        <v>134</v>
+      </c>
+      <c r="M23" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23">
-        <v>21</v>
-      </c>
-      <c r="I23">
-        <v>30</v>
-      </c>
-      <c r="J23">
-        <v>29</v>
-      </c>
-      <c r="K23" t="s">
-        <v>133</v>
-      </c>
-      <c r="L23" t="s">
-        <v>129</v>
-      </c>
-      <c r="M23">
+      <c r="N23">
         <v>4</v>
       </c>
-      <c r="N23" t="s">
-        <v>117</v>
-      </c>
       <c r="O23" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="P23" t="s">
-        <v>134</v>
+        <v>47</v>
       </c>
       <c r="Q23" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" t="s">
         <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I24">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>139</v>
+      </c>
+      <c r="J24">
         <v>1</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>2</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>5</v>
       </c>
-      <c r="P24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>141</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>143</v>
+      </c>
+      <c r="I25">
         <v>16</v>
       </c>
-      <c r="L25" t="s">
-        <v>106</v>
-      </c>
-      <c r="M25">
+      <c r="M25" t="s">
+        <v>108</v>
+      </c>
+      <c r="N25">
         <v>5</v>
       </c>
-      <c r="O25" t="s">
-        <v>38</v>
-      </c>
       <c r="P25" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q25" t="s">
-        <v>143</v>
+        <v>28</v>
       </c>
       <c r="R25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="S25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26">
+        <v>31</v>
+      </c>
+      <c r="G26" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26">
         <v>24</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>16</v>
       </c>
-      <c r="K26" t="s">
-        <v>147</v>
-      </c>
-      <c r="M26">
+      <c r="L26" t="s">
+        <v>148</v>
+      </c>
+      <c r="N26">
         <v>6</v>
       </c>
-      <c r="O26" t="s">
-        <v>38</v>
-      </c>
       <c r="P26" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q26" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="R26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="S26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I27">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>152</v>
+      </c>
+      <c r="J27">
         <v>24</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>16</v>
       </c>
-      <c r="K27" t="s">
-        <v>152</v>
-      </c>
-      <c r="M27">
+      <c r="L27" t="s">
+        <v>153</v>
+      </c>
+      <c r="N27">
         <v>6</v>
       </c>
-      <c r="O27" t="s">
-        <v>38</v>
-      </c>
       <c r="P27" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q27" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="R27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="S27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" t="s">
         <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="G28" t="s">
         <v>157</v>
       </c>
-      <c r="H28">
-        <v>28</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="H28" t="s">
         <v>158</v>
       </c>
-      <c r="M28">
+      <c r="I28">
+        <v>28</v>
+      </c>
+      <c r="M28" t="s">
+        <v>159</v>
+      </c>
+      <c r="N28">
         <v>3</v>
-      </c>
-      <c r="N28" t="s">
-        <v>159</v>
       </c>
       <c r="O28" t="s">
         <v>160</v>
       </c>
       <c r="P28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="F29" t="s">
-        <v>164</v>
+        <v>31</v>
       </c>
       <c r="G29" t="s">
         <v>165</v>
       </c>
-      <c r="H29">
+      <c r="H29" t="s">
+        <v>166</v>
+      </c>
+      <c r="I29">
         <v>27</v>
       </c>
-      <c r="L29" t="s">
-        <v>158</v>
-      </c>
-      <c r="M29">
+      <c r="M29" t="s">
+        <v>159</v>
+      </c>
+      <c r="N29">
         <v>3</v>
       </c>
-      <c r="O29" t="s">
-        <v>166</v>
-      </c>
       <c r="P29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="E30" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30">
         <v>30</v>
       </c>
-      <c r="F30" t="s">
-        <v>169</v>
-      </c>
-      <c r="G30" t="s">
-        <v>170</v>
-      </c>
-      <c r="H30">
-        <v>30</v>
-      </c>
-      <c r="I30">
+      <c r="J30">
         <v>32</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>31</v>
       </c>
-      <c r="K30" t="s">
-        <v>171</v>
-      </c>
       <c r="L30" t="s">
-        <v>172</v>
-      </c>
-      <c r="M30">
+        <v>173</v>
+      </c>
+      <c r="M30" t="s">
+        <v>174</v>
+      </c>
+      <c r="N30">
         <v>3</v>
       </c>
-      <c r="N30" t="s">
-        <v>173</v>
-      </c>
-      <c r="P30" t="s">
-        <v>27</v>
+      <c r="O30" t="s">
+        <v>175</v>
       </c>
       <c r="Q30" t="s">
-        <v>174</v>
+        <v>28</v>
       </c>
       <c r="R30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="S30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="F31" t="s">
-        <v>177</v>
+        <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>178</v>
-      </c>
-      <c r="H31">
+        <v>179</v>
+      </c>
+      <c r="H31" t="s">
+        <v>180</v>
+      </c>
+      <c r="I31">
         <v>29</v>
       </c>
-      <c r="L31" t="s">
-        <v>172</v>
-      </c>
-      <c r="M31">
+      <c r="M31" t="s">
+        <v>174</v>
+      </c>
+      <c r="N31">
         <v>3</v>
       </c>
-      <c r="N31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
-      </c>
-      <c r="E32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32">
+        <v>184</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32">
         <v>1894</v>
       </c>
-      <c r="G32" t="s">
-        <v>165</v>
-      </c>
-      <c r="H32">
+      <c r="H32" t="s">
+        <v>166</v>
+      </c>
+      <c r="I32">
         <v>32</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>59</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>60</v>
       </c>
       <c r="L32" t="s">
-        <v>183</v>
-      </c>
-      <c r="M32">
+        <v>185</v>
+      </c>
+      <c r="M32" t="s">
+        <v>186</v>
+      </c>
+      <c r="N32">
         <v>2</v>
       </c>
-      <c r="P32" t="s">
-        <v>27</v>
-      </c>
       <c r="Q32" t="s">
-        <v>184</v>
+        <v>28</v>
       </c>
       <c r="R32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="S32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <v>1897</v>
+      </c>
+      <c r="H33">
+        <v>1942</v>
+      </c>
+      <c r="I33">
+        <v>31</v>
+      </c>
+      <c r="J33">
+        <v>51</v>
+      </c>
+      <c r="K33">
+        <v>58</v>
+      </c>
+      <c r="L33" t="s">
+        <v>190</v>
+      </c>
+      <c r="M33" t="s">
         <v>186</v>
       </c>
-      <c r="D33" t="s">
-        <v>187</v>
-      </c>
-      <c r="E33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33">
-        <v>1897</v>
-      </c>
-      <c r="G33" t="s">
-        <v>165</v>
-      </c>
-      <c r="H33">
-        <v>31</v>
-      </c>
-      <c r="I33">
-        <v>51</v>
-      </c>
-      <c r="J33">
-        <v>58</v>
-      </c>
-      <c r="K33" t="s">
-        <v>188</v>
-      </c>
-      <c r="L33" t="s">
-        <v>183</v>
-      </c>
-      <c r="M33">
+      <c r="N33">
         <v>2</v>
       </c>
-      <c r="P33" t="s">
-        <v>27</v>
-      </c>
       <c r="Q33" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34">
+        <v>170</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34">
         <v>1923</v>
       </c>
-      <c r="H34">
+      <c r="H34" t="s">
+        <v>324</v>
+      </c>
+      <c r="I34">
         <v>36</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>32</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>31</v>
       </c>
-      <c r="K34" t="s">
-        <v>191</v>
-      </c>
       <c r="L34" t="s">
-        <v>192</v>
-      </c>
-      <c r="M34">
+        <v>193</v>
+      </c>
+      <c r="M34" t="s">
+        <v>194</v>
+      </c>
+      <c r="N34">
         <v>3</v>
       </c>
-      <c r="P34" t="s">
-        <v>193</v>
-      </c>
       <c r="Q34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="R34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="S34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="F35" t="s">
-        <v>196</v>
+        <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>165</v>
-      </c>
-      <c r="H35">
+        <v>198</v>
+      </c>
+      <c r="H35" t="s">
+        <v>166</v>
+      </c>
+      <c r="I35">
         <v>38</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>32</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>31</v>
       </c>
-      <c r="K35" t="s">
-        <v>197</v>
-      </c>
       <c r="L35" t="s">
-        <v>198</v>
-      </c>
-      <c r="M35">
+        <v>199</v>
+      </c>
+      <c r="M35" t="s">
+        <v>200</v>
+      </c>
+      <c r="N35">
         <v>3</v>
       </c>
-      <c r="O35" t="s">
-        <v>199</v>
-      </c>
       <c r="P35" t="s">
-        <v>27</v>
+        <v>201</v>
       </c>
       <c r="Q35" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="R35" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="S35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
+        <v>170</v>
       </c>
       <c r="F36" t="s">
-        <v>202</v>
-      </c>
-      <c r="H36">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>204</v>
+      </c>
+      <c r="H36" t="s">
+        <v>166</v>
+      </c>
+      <c r="I36">
         <v>44</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>32</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>31</v>
       </c>
-      <c r="K36" t="s">
-        <v>203</v>
-      </c>
       <c r="L36" t="s">
-        <v>204</v>
-      </c>
-      <c r="M36">
+        <v>205</v>
+      </c>
+      <c r="M36" t="s">
+        <v>206</v>
+      </c>
+      <c r="N36">
         <v>3</v>
       </c>
-      <c r="O36" t="s">
-        <v>38</v>
-      </c>
       <c r="P36" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q36" t="s">
-        <v>205</v>
+        <v>28</v>
       </c>
       <c r="R36" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="S36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
-      </c>
-      <c r="E37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37">
+        <v>170</v>
+      </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37">
         <v>33</v>
       </c>
-      <c r="L37" t="s">
-        <v>192</v>
-      </c>
-      <c r="M37">
+      <c r="M37" t="s">
+        <v>194</v>
+      </c>
+      <c r="N37">
         <v>3</v>
       </c>
-      <c r="O37" t="s">
-        <v>38</v>
-      </c>
       <c r="P37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
-      </c>
-      <c r="E38" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38">
+        <v>170</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38">
         <v>53</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>33</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>36</v>
       </c>
-      <c r="L38" t="s">
-        <v>210</v>
-      </c>
-      <c r="M38">
+      <c r="M38" t="s">
+        <v>212</v>
+      </c>
+      <c r="N38">
         <v>4</v>
       </c>
-      <c r="O38" t="s">
-        <v>211</v>
-      </c>
       <c r="P38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C39" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D39" t="s">
-        <v>214</v>
-      </c>
-      <c r="E39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G39" t="s">
-        <v>165</v>
-      </c>
-      <c r="H39">
+        <v>216</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39">
         <v>34</v>
       </c>
-      <c r="L39" t="s">
-        <v>198</v>
-      </c>
-      <c r="M39">
+      <c r="M39" t="s">
+        <v>200</v>
+      </c>
+      <c r="N39">
         <v>3</v>
       </c>
-      <c r="N39" t="s">
-        <v>215</v>
-      </c>
       <c r="O39" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="P39" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="Q39" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="R39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D40" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>197</v>
       </c>
       <c r="F40" t="s">
-        <v>221</v>
-      </c>
-      <c r="H40">
+        <v>31</v>
+      </c>
+      <c r="G40" t="s">
+        <v>223</v>
+      </c>
+      <c r="I40">
         <v>40</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>38</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>34</v>
       </c>
-      <c r="K40" t="s">
-        <v>222</v>
-      </c>
       <c r="L40" t="s">
-        <v>223</v>
-      </c>
-      <c r="M40">
+        <v>224</v>
+      </c>
+      <c r="M40" t="s">
+        <v>225</v>
+      </c>
+      <c r="N40">
         <v>4</v>
       </c>
-      <c r="O40" t="s">
-        <v>224</v>
-      </c>
       <c r="P40" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="Q40" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R40" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>228</v>
+      </c>
+      <c r="C41" t="s">
+        <v>229</v>
+      </c>
+      <c r="D41" t="s">
+        <v>230</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41">
+        <v>39</v>
+      </c>
+      <c r="M41" t="s">
+        <v>225</v>
+      </c>
+      <c r="N41">
+        <v>4</v>
+      </c>
+      <c r="P41" t="s">
         <v>226</v>
       </c>
-      <c r="C41" t="s">
-        <v>227</v>
-      </c>
-      <c r="D41" t="s">
-        <v>228</v>
-      </c>
-      <c r="E41" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41">
-        <v>39</v>
-      </c>
-      <c r="L41" t="s">
-        <v>223</v>
-      </c>
-      <c r="M41">
-        <v>4</v>
-      </c>
-      <c r="O41" t="s">
-        <v>224</v>
-      </c>
-      <c r="P41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D42" t="s">
         <v>230</v>
       </c>
-      <c r="D42" t="s">
-        <v>228</v>
-      </c>
-      <c r="E42" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42">
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42">
         <v>40</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>39</v>
       </c>
-      <c r="K42" t="s">
-        <v>231</v>
-      </c>
-      <c r="M42">
+      <c r="L42" t="s">
+        <v>233</v>
+      </c>
+      <c r="N42">
         <v>5</v>
       </c>
-      <c r="O42" t="s">
-        <v>224</v>
-      </c>
       <c r="P42" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="Q42" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R42" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C43" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D43" t="s">
-        <v>228</v>
-      </c>
-      <c r="E43" t="s">
-        <v>21</v>
-      </c>
-      <c r="I43">
+        <v>230</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="J43">
         <v>57</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>43</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>6</v>
       </c>
-      <c r="O43" t="s">
-        <v>224</v>
-      </c>
       <c r="P43" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
       <c r="Q43" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C44" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D44" t="s">
-        <v>238</v>
-      </c>
-      <c r="E44" t="s">
-        <v>30</v>
-      </c>
-      <c r="H44">
+        <v>240</v>
+      </c>
+      <c r="F44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44">
         <v>57</v>
       </c>
-      <c r="L44" t="s">
-        <v>239</v>
-      </c>
-      <c r="M44">
+      <c r="M44" t="s">
+        <v>241</v>
+      </c>
+      <c r="N44">
         <v>5</v>
       </c>
-      <c r="O44" t="s">
-        <v>224</v>
-      </c>
       <c r="P44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C45" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
-      </c>
-      <c r="E45" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="F45" t="s">
-        <v>242</v>
-      </c>
-      <c r="H45">
+        <v>31</v>
+      </c>
+      <c r="G45" t="s">
+        <v>244</v>
+      </c>
+      <c r="I45">
         <v>35</v>
       </c>
-      <c r="L45" t="s">
-        <v>204</v>
-      </c>
-      <c r="M45">
+      <c r="M45" t="s">
+        <v>206</v>
+      </c>
+      <c r="N45">
         <v>3</v>
       </c>
-      <c r="O45" t="s">
-        <v>38</v>
-      </c>
       <c r="P45" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C46" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D46" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E46" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="F46" t="s">
-        <v>246</v>
-      </c>
-      <c r="H46">
+        <v>31</v>
+      </c>
+      <c r="G46" t="s">
+        <v>248</v>
+      </c>
+      <c r="I46">
         <v>48</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>35</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>44</v>
       </c>
-      <c r="K46" t="s">
-        <v>247</v>
-      </c>
       <c r="L46" t="s">
-        <v>248</v>
-      </c>
-      <c r="M46">
+        <v>249</v>
+      </c>
+      <c r="M46" t="s">
+        <v>250</v>
+      </c>
+      <c r="N46">
         <v>4</v>
       </c>
-      <c r="O46" t="s">
-        <v>38</v>
-      </c>
       <c r="P46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C47" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D47" t="s">
-        <v>187</v>
-      </c>
-      <c r="E47" t="s">
-        <v>21</v>
+        <v>170</v>
       </c>
       <c r="F47" t="s">
-        <v>251</v>
-      </c>
-      <c r="I47">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>253</v>
+      </c>
+      <c r="J47">
         <v>35</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>44</v>
       </c>
-      <c r="K47" t="s">
-        <v>252</v>
-      </c>
       <c r="L47" t="s">
-        <v>253</v>
-      </c>
-      <c r="M47">
+        <v>254</v>
+      </c>
+      <c r="M47" t="s">
+        <v>255</v>
+      </c>
+      <c r="N47">
         <v>4</v>
       </c>
-      <c r="O47" t="s">
-        <v>38</v>
-      </c>
       <c r="P47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>255</v>
-      </c>
-      <c r="E48" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" t="s">
-        <v>256</v>
-      </c>
-      <c r="I48">
+        <v>257</v>
+      </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" t="s">
+        <v>258</v>
+      </c>
+      <c r="J48">
         <v>48</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>45</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>5</v>
       </c>
-      <c r="O48" t="s">
-        <v>38</v>
-      </c>
       <c r="P48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C49" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D49" t="s">
-        <v>255</v>
-      </c>
-      <c r="E49" t="s">
-        <v>21</v>
-      </c>
-      <c r="H49">
+        <v>257</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49">
         <v>45</v>
       </c>
-      <c r="L49" t="s">
-        <v>248</v>
-      </c>
-      <c r="M49">
+      <c r="M49" t="s">
+        <v>250</v>
+      </c>
+      <c r="N49">
         <v>4</v>
       </c>
-      <c r="O49" t="s">
-        <v>38</v>
-      </c>
       <c r="P49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" t="s">
         <v>30</v>
       </c>
-      <c r="I50">
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+      <c r="J50">
         <v>46</v>
       </c>
-      <c r="K50" t="s">
-        <v>257</v>
-      </c>
-      <c r="M50">
+      <c r="L50" t="s">
+        <v>259</v>
+      </c>
+      <c r="N50">
         <v>5</v>
       </c>
-      <c r="P50" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q50" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C51" t="s">
-        <v>260</v>
-      </c>
-      <c r="E51" t="s">
-        <v>21</v>
-      </c>
-      <c r="I51">
+        <v>262</v>
+      </c>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
+      <c r="J51">
         <v>46</v>
       </c>
-      <c r="K51" t="s">
-        <v>261</v>
-      </c>
-      <c r="M51">
+      <c r="L51" t="s">
+        <v>263</v>
+      </c>
+      <c r="N51">
         <v>5</v>
       </c>
-      <c r="O51" t="s">
-        <v>262</v>
-      </c>
       <c r="P51" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C52" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D52" t="s">
-        <v>187</v>
-      </c>
-      <c r="E52" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52">
+        <v>170</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52">
         <v>1867</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>1937</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>58</v>
       </c>
-      <c r="L52" t="s">
-        <v>266</v>
-      </c>
-      <c r="M52">
+      <c r="M52" t="s">
+        <v>268</v>
+      </c>
+      <c r="N52">
         <v>1</v>
       </c>
-      <c r="O52" t="s">
-        <v>267</v>
-      </c>
       <c r="P52" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="Q52" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="R52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D53" t="s">
-        <v>187</v>
-      </c>
-      <c r="E53" t="s">
-        <v>21</v>
-      </c>
-      <c r="G53" t="s">
-        <v>165</v>
-      </c>
-      <c r="I53">
+        <v>170</v>
+      </c>
+      <c r="F53" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" t="s">
+        <v>166</v>
+      </c>
+      <c r="J53">
         <v>51</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>58</v>
       </c>
-      <c r="K53" t="s">
-        <v>270</v>
-      </c>
-      <c r="M53">
+      <c r="L53" t="s">
+        <v>272</v>
+      </c>
+      <c r="N53">
         <v>2</v>
       </c>
-      <c r="O53" t="s">
-        <v>38</v>
-      </c>
       <c r="P53" t="s">
-        <v>271</v>
+        <v>39</v>
       </c>
       <c r="Q53" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="R53" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C54" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
-      </c>
-      <c r="E54" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54">
+        <v>170</v>
+      </c>
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54">
         <v>37</v>
       </c>
-      <c r="L54" t="s">
-        <v>210</v>
-      </c>
-      <c r="M54">
+      <c r="M54" t="s">
+        <v>212</v>
+      </c>
+      <c r="N54">
         <v>4</v>
       </c>
-      <c r="O54" t="s">
-        <v>38</v>
-      </c>
       <c r="P54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" t="s">
-        <v>21</v>
-      </c>
-      <c r="I55">
+        <v>141</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55">
         <v>37</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>53</v>
       </c>
-      <c r="K55" t="s">
-        <v>275</v>
-      </c>
-      <c r="M55">
+      <c r="L55" t="s">
+        <v>277</v>
+      </c>
+      <c r="N55">
         <v>5</v>
       </c>
-      <c r="P55" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C56" t="s">
-        <v>277</v>
-      </c>
-      <c r="E56" t="s">
-        <v>21</v>
-      </c>
-      <c r="I56">
+        <v>279</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56">
         <v>37</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>53</v>
       </c>
-      <c r="K56" t="s">
-        <v>278</v>
-      </c>
-      <c r="M56">
+      <c r="L56" t="s">
+        <v>280</v>
+      </c>
+      <c r="N56">
         <v>5</v>
       </c>
-      <c r="P56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C57" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D57" t="s">
-        <v>214</v>
-      </c>
-      <c r="E57" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57">
+        <v>216</v>
+      </c>
+      <c r="F57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J57">
         <v>38</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>34</v>
       </c>
-      <c r="K57" t="s">
-        <v>281</v>
-      </c>
-      <c r="M57">
+      <c r="L57" t="s">
+        <v>283</v>
+      </c>
+      <c r="N57">
         <v>4</v>
       </c>
-      <c r="O57" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>228</v>
+      </c>
+      <c r="C58" t="s">
+        <v>229</v>
+      </c>
+      <c r="D58" t="s">
+        <v>230</v>
+      </c>
+      <c r="F58" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58">
+        <v>43</v>
+      </c>
+      <c r="J58">
+        <v>40</v>
+      </c>
+      <c r="K58">
+        <v>39</v>
+      </c>
+      <c r="L58" t="s">
+        <v>284</v>
+      </c>
+      <c r="M58" t="s">
+        <v>241</v>
+      </c>
+      <c r="N58">
+        <v>5</v>
+      </c>
+      <c r="P58" t="s">
         <v>226</v>
       </c>
-      <c r="C58" t="s">
-        <v>227</v>
-      </c>
-      <c r="D58" t="s">
-        <v>228</v>
-      </c>
-      <c r="E58" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58">
-        <v>43</v>
-      </c>
-      <c r="I58">
-        <v>40</v>
-      </c>
-      <c r="J58">
-        <v>39</v>
-      </c>
-      <c r="K58" t="s">
-        <v>282</v>
-      </c>
-      <c r="L58" t="s">
-        <v>239</v>
-      </c>
-      <c r="M58">
-        <v>5</v>
-      </c>
-      <c r="O58" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C59" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D59" t="s">
-        <v>187</v>
-      </c>
-      <c r="E59" t="s">
-        <v>30</v>
-      </c>
-      <c r="H59">
+        <v>170</v>
+      </c>
+      <c r="F59" t="s">
+        <v>31</v>
+      </c>
+      <c r="I59">
         <v>51</v>
       </c>
-      <c r="L59" t="s">
-        <v>266</v>
-      </c>
-      <c r="M59">
+      <c r="M59" t="s">
+        <v>268</v>
+      </c>
+      <c r="N59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C60" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D60" t="s">
-        <v>288</v>
-      </c>
-      <c r="E60" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60">
+        <v>290</v>
+      </c>
+      <c r="F60" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60">
         <v>60</v>
       </c>
-      <c r="L60" t="s">
-        <v>289</v>
-      </c>
-      <c r="M60">
+      <c r="M60" t="s">
+        <v>291</v>
+      </c>
+      <c r="N60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>292</v>
+      </c>
+      <c r="C61" t="s">
+        <v>293</v>
+      </c>
+      <c r="D61" t="s">
+        <v>184</v>
+      </c>
+      <c r="F61" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61">
+        <v>59</v>
+      </c>
+      <c r="M61" t="s">
+        <v>291</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>294</v>
+      </c>
+      <c r="C62" t="s">
+        <v>295</v>
+      </c>
+      <c r="D62" t="s">
+        <v>170</v>
+      </c>
+      <c r="F62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62">
+        <v>1880</v>
+      </c>
+      <c r="H62" t="s">
+        <v>166</v>
+      </c>
+      <c r="J62">
+        <v>51</v>
+      </c>
+      <c r="K62">
+        <v>58</v>
+      </c>
+      <c r="L62" t="s">
+        <v>296</v>
+      </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>297</v>
+      </c>
+      <c r="C63" t="s">
+        <v>298</v>
+      </c>
+      <c r="D63" t="s">
+        <v>170</v>
+      </c>
+      <c r="F63" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63">
+        <v>1886</v>
+      </c>
+      <c r="H63">
+        <v>1942</v>
+      </c>
+      <c r="J63">
+        <v>51</v>
+      </c>
+      <c r="K63">
+        <v>58</v>
+      </c>
+      <c r="L63" t="s">
+        <v>299</v>
+      </c>
+      <c r="N63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>300</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" t="s">
+        <v>170</v>
+      </c>
+      <c r="F64" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64">
+        <v>1904</v>
+      </c>
+      <c r="H64" t="s">
+        <v>166</v>
+      </c>
+      <c r="J64">
+        <v>51</v>
+      </c>
+      <c r="K64">
+        <v>58</v>
+      </c>
+      <c r="L64" t="s">
+        <v>301</v>
+      </c>
+      <c r="N64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>302</v>
+      </c>
+      <c r="C65" t="s">
+        <v>303</v>
+      </c>
+      <c r="D65" t="s">
+        <v>170</v>
+      </c>
+      <c r="F65" t="s">
+        <v>31</v>
+      </c>
+      <c r="G65">
+        <v>1883</v>
+      </c>
+      <c r="H65" t="s">
+        <v>166</v>
+      </c>
+      <c r="J65">
+        <v>51</v>
+      </c>
+      <c r="K65">
+        <v>58</v>
+      </c>
+      <c r="L65" t="s">
+        <v>304</v>
+      </c>
+      <c r="N65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>305</v>
+      </c>
+      <c r="C66" t="s">
+        <v>306</v>
+      </c>
+      <c r="D66" t="s">
+        <v>170</v>
+      </c>
+      <c r="F66" t="s">
+        <v>31</v>
+      </c>
+      <c r="G66">
+        <v>1895</v>
+      </c>
+      <c r="H66" t="s">
+        <v>166</v>
+      </c>
+      <c r="J66">
+        <v>51</v>
+      </c>
+      <c r="K66">
+        <v>58</v>
+      </c>
+      <c r="L66" t="s">
+        <v>307</v>
+      </c>
+      <c r="N66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>308</v>
+      </c>
+      <c r="C67" t="s">
+        <v>309</v>
+      </c>
+      <c r="D67" t="s">
         <v>290</v>
       </c>
-      <c r="C61" t="s">
-        <v>291</v>
-      </c>
-      <c r="D61" t="s">
-        <v>182</v>
-      </c>
-      <c r="E61" t="s">
-        <v>30</v>
-      </c>
-      <c r="H61">
+      <c r="F67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" t="s">
+        <v>166</v>
+      </c>
+      <c r="J67">
         <v>59</v>
       </c>
-      <c r="L61" t="s">
-        <v>289</v>
-      </c>
-      <c r="M61">
-        <v>1</v>
+      <c r="K67">
+        <v>60</v>
+      </c>
+      <c r="L67" t="s">
+        <v>310</v>
+      </c>
+      <c r="N67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" t="s">
+        <v>290</v>
+      </c>
+      <c r="F68" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" t="s">
+        <v>166</v>
+      </c>
+      <c r="J68">
+        <v>59</v>
+      </c>
+      <c r="K68">
+        <v>60</v>
+      </c>
+      <c r="L68" t="s">
+        <v>311</v>
+      </c>
+      <c r="N68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>312</v>
+      </c>
+      <c r="C69" t="s">
+        <v>313</v>
+      </c>
+      <c r="D69" t="s">
+        <v>314</v>
+      </c>
+      <c r="E69" t="s">
+        <v>184</v>
+      </c>
+      <c r="F69" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69" t="s">
+        <v>166</v>
+      </c>
+      <c r="H69">
+        <v>1943</v>
+      </c>
+      <c r="J69">
+        <v>59</v>
+      </c>
+      <c r="K69">
+        <v>60</v>
+      </c>
+      <c r="L69" t="s">
+        <v>315</v>
+      </c>
+      <c r="N69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>316</v>
+      </c>
+      <c r="C70" t="s">
+        <v>317</v>
+      </c>
+      <c r="D70" t="s">
+        <v>318</v>
+      </c>
+      <c r="E70" t="s">
+        <v>184</v>
+      </c>
+      <c r="F70" t="s">
+        <v>31</v>
+      </c>
+      <c r="H70" t="s">
+        <v>166</v>
+      </c>
+      <c r="J70">
+        <v>59</v>
+      </c>
+      <c r="K70">
+        <v>60</v>
+      </c>
+      <c r="L70" t="s">
+        <v>319</v>
+      </c>
+      <c r="N70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>320</v>
+      </c>
+      <c r="C71" t="s">
+        <v>321</v>
+      </c>
+      <c r="D71" t="s">
+        <v>322</v>
+      </c>
+      <c r="E71" t="s">
+        <v>184</v>
+      </c>
+      <c r="F71" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" t="s">
+        <v>166</v>
+      </c>
+      <c r="H71">
+        <v>1942</v>
+      </c>
+      <c r="J71">
+        <v>59</v>
+      </c>
+      <c r="K71">
+        <v>60</v>
+      </c>
+      <c r="L71" t="s">
+        <v>323</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>